<commit_message>
putting timings into report + tiny refactor
</commit_message>
<xml_diff>
--- a/part-2/Docs/Timings.xlsx
+++ b/part-2/Docs/Timings.xlsx
@@ -492,6 +492,44 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Radius</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.4547088880822116"/>
+              <c:y val="0.85297317110661797"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1158,6 +1196,44 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Radius</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45963684393637733"/>
+              <c:y val="0.85846195750369925"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1857,6 +1933,44 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Radius</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45353458581591966"/>
+              <c:y val="0.86256331865488378"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2524,6 +2638,39 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blur Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45937959097394704"/>
+              <c:y val="0.8643669380167126"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5448,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>